<commit_message>
eqtl colocalisation for final credset July2025
</commit_message>
<xml_diff>
--- a/src/report/locus2gene.xlsx
+++ b/src/report/locus2gene.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\PhD\PhD_project\Var_to_Gene\src\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4F58E7-13F0-432D-BED2-283BE133CA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2DFFDA-33A8-47FB-9E80-B0710600CA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13215" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="L2G_clean" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="L2G_clean_noMHC_chr3" sheetId="4" r:id="rId1"/>
+    <sheet name="L2G_clean" sheetId="2" r:id="rId2"/>
+    <sheet name="L2G_clean_chr3_rs778801698" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$B$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet1!$A$1:$B$123</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="142">
   <si>
     <t>locus</t>
   </si>
@@ -383,6 +385,78 @@
   </si>
   <si>
     <t>TPD52</t>
+  </si>
+  <si>
+    <t>3_rs778801698_49524027_50524027</t>
+  </si>
+  <si>
+    <t>RNF123</t>
+  </si>
+  <si>
+    <t>IP6K1</t>
+  </si>
+  <si>
+    <t>MST1</t>
+  </si>
+  <si>
+    <t>SHISA5</t>
+  </si>
+  <si>
+    <t>TDGF1</t>
+  </si>
+  <si>
+    <t>UBA7</t>
+  </si>
+  <si>
+    <t>TRAIP</t>
+  </si>
+  <si>
+    <t>MST1R</t>
+  </si>
+  <si>
+    <t>MON1A</t>
+  </si>
+  <si>
+    <t>RBM6</t>
+  </si>
+  <si>
+    <t>CACNA2D2</t>
+  </si>
+  <si>
+    <t>CYB561D2</t>
+  </si>
+  <si>
+    <t>GNAI2</t>
+  </si>
+  <si>
+    <t>ZMYND10</t>
+  </si>
+  <si>
+    <t>NARS1</t>
+  </si>
+  <si>
+    <t>PRKAR2A</t>
+  </si>
+  <si>
+    <t>SEMA3F-AS1</t>
+  </si>
+  <si>
+    <t>GMPPB</t>
+  </si>
+  <si>
+    <t>CAMKV</t>
+  </si>
+  <si>
+    <t>RBM5</t>
+  </si>
+  <si>
+    <t>HYAL3</t>
+  </si>
+  <si>
+    <t>NAA80</t>
+  </si>
+  <si>
+    <t>IL1RL1/ST2</t>
   </si>
 </sst>
 </file>
@@ -432,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -445,6 +519,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -725,14 +802,933 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC502C4-6FB0-48CD-8038-AEB9C3FAADD9}">
+  <dimension ref="A1:B112"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="45.36328125" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>20</v>
+      </c>
+      <c r="B76" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>34</v>
+      </c>
+      <c r="B78" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>34</v>
+      </c>
+      <c r="B79" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>34</v>
+      </c>
+      <c r="B80" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>38</v>
+      </c>
+      <c r="B81" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>38</v>
+      </c>
+      <c r="B83" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>41</v>
+      </c>
+      <c r="B84" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>41</v>
+      </c>
+      <c r="B85" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>41</v>
+      </c>
+      <c r="B86" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>41</v>
+      </c>
+      <c r="B87" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>41</v>
+      </c>
+      <c r="B88" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>41</v>
+      </c>
+      <c r="B89" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>41</v>
+      </c>
+      <c r="B90" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>118</v>
+      </c>
+      <c r="B91" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>118</v>
+      </c>
+      <c r="B92" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>118</v>
+      </c>
+      <c r="B93" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>118</v>
+      </c>
+      <c r="B94" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>118</v>
+      </c>
+      <c r="B95" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>118</v>
+      </c>
+      <c r="B96" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>118</v>
+      </c>
+      <c r="B97" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>118</v>
+      </c>
+      <c r="B98" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>118</v>
+      </c>
+      <c r="B99" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>118</v>
+      </c>
+      <c r="B100" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>118</v>
+      </c>
+      <c r="B101" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>118</v>
+      </c>
+      <c r="B102" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>118</v>
+      </c>
+      <c r="B103" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>118</v>
+      </c>
+      <c r="B104" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>118</v>
+      </c>
+      <c r="B105" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>118</v>
+      </c>
+      <c r="B106" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>118</v>
+      </c>
+      <c r="B107" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>118</v>
+      </c>
+      <c r="B108" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>118</v>
+      </c>
+      <c r="B109" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>118</v>
+      </c>
+      <c r="B110" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>118</v>
+      </c>
+      <c r="B111" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>118</v>
+      </c>
+      <c r="B112" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC84B80-4315-4F3E-9D19-D47758DB5717}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="45.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1539,7 +2535,210 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71133EF5-737E-4ED5-B28A-752A0CDDCF0E}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="A2:B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="19.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:B123"/>

</xml_diff>